<commit_message>
tlt-2560: selenium tests - manage sections permissions - only includes two test roles (yes/no) in colgsas for now; more data can be added later
</commit_message>
<xml_diff>
--- a/selenium_tests/manage_sections/test_data/permissions_roles_access.xlsx
+++ b/selenium_tests/manage_sections/test_data/permissions_roles_access.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ely817/tlt/canvas_manage_course/selenium_tests/manage_sections/test_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="testing_access" sheetId="1" r:id="rId1"/>
     <sheet name="Site Setup" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -21,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t xml:space="preserve">Roles </t>
   </si>
@@ -29,15 +36,6 @@
     <t xml:space="preserve">Masquerade ID </t>
   </si>
   <si>
-    <t xml:space="preserve">Guest </t>
-  </si>
-  <si>
-    <t>Harvard-Viewer</t>
-  </si>
-  <si>
-    <t>Observer</t>
-  </si>
-  <si>
     <t>given_access</t>
   </si>
   <si>
@@ -47,72 +45,12 @@
     <t>test15@mcelroy.org</t>
   </si>
   <si>
-    <t>test16@mcelroy.org</t>
-  </si>
-  <si>
-    <t>test2@mcelroy.org</t>
-  </si>
-  <si>
-    <t>test3@mcelroy.org</t>
-  </si>
-  <si>
-    <t>test5@mcelroy.org</t>
-  </si>
-  <si>
     <t>TA</t>
   </si>
   <si>
-    <t xml:space="preserve">Teaching Staff </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Course Head </t>
-  </si>
-  <si>
-    <t>Course Support Staff</t>
-  </si>
-  <si>
-    <t>Course Designer</t>
-  </si>
-  <si>
-    <t>test11@mcelroy.org</t>
-  </si>
-  <si>
-    <t>test80@mcelroy.org</t>
-  </si>
-  <si>
-    <t>tlttest54@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Course or Account Level Roles </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes </t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t xml:space="preserve">No </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Account admin </t>
-  </si>
-  <si>
-    <t>School Liaison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Account Level Role (sub-account 10) </t>
-  </si>
-  <si>
-    <t>Account Level Role (sub-account 10)</t>
-  </si>
-  <si>
-    <t>test7@mcelroy.org</t>
-  </si>
-  <si>
-    <t>test8@mcelroy.org</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -122,28 +60,37 @@
     <t xml:space="preserve">canvas_user_id </t>
   </si>
   <si>
-    <t>Access to CLASS ROSTER</t>
-  </si>
-  <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Course Level Role (course 3787) </t>
-  </si>
-  <si>
     <t xml:space="preserve">Site Under Test </t>
   </si>
   <si>
-    <t>https://canvas.dev.tlt.harvard.edu/courses/3787/external_tools/162</t>
-  </si>
-  <si>
     <t xml:space="preserve">Test Data Info: </t>
   </si>
   <si>
     <t>https://confluence.huit.harvard.edu/display/TLT/SIS+Import+of+Test+Data+for+Selenium+Permissions+Test</t>
   </si>
   <si>
-    <t>92234</t>
+    <t>expected_role</t>
+  </si>
+  <si>
+    <t>92259</t>
+  </si>
+  <si>
+    <t>Librarian</t>
+  </si>
+  <si>
+    <t>Access to course 27 manage sections</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>test35@mcelroy.org</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>https://canvas.dev.tlt.harvard.edu/courses/27/external_tools/195</t>
   </si>
 </sst>
 </file>
@@ -221,7 +168,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="163">
+  <cellStyleXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -385,8 +332,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -396,8 +344,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="129" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="129"/>
   </cellXfs>
-  <cellStyles count="163">
+  <cellStyles count="164">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -495,6 +444,7 @@
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -564,6 +514,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -889,62 +844,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.1640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="31" style="4" customWidth="1"/>
@@ -954,251 +914,104 @@
     <col min="6" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C2" s="4">
         <v>92241</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="C3" s="4">
-        <v>92242</v>
+        <v>92259</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4">
-        <v>92229</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4">
-        <v>92230</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="6" t="s">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="4">
-        <v>92232</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="4">
-        <v>92295</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="4">
-        <v>90670</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="4">
-        <v>92238</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="4">
-        <v>92234</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="4">
-        <v>92235</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B11" r:id="rId8"/>
-    <hyperlink ref="B12" r:id="rId9"/>
-    <hyperlink ref="B9" r:id="rId10"/>
+    <hyperlink ref="A15" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>